<commit_message>
Updated test data for TC 203, 205,41,51822
</commit_message>
<xml_diff>
--- a/Test Data/TC_203_Verify_If_An_EXI800_Is_Deleted_All_The_IS_Devices_Connected_To_EXI800_Will_Be_Deleted.xlsx
+++ b/Test Data/TC_203_Verify_If_An_EXI800_Is_Deleted_All_The_IS_Devices_Connected_To_EXI800_Will_Be_Deleted.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdhakaa\Documents\NG Consys Project\Testing\NGConsys Automation\Test Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A868762E-C6FF-4A2A-9313-04ABC3AF8D67}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84383E08-6B72-4DAD-8F50-9FC95DA3B7EA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Add EXI Devices" sheetId="6" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="40">
   <si>
     <t>Color Codes</t>
   </si>
@@ -153,24 +153,6 @@
   </si>
   <si>
     <t>VerifyConnectedISDevicesOnEXI</t>
-  </si>
-  <si>
-    <t>0 / 1</t>
-  </si>
-  <si>
-    <t>0 / 2</t>
-  </si>
-  <si>
-    <t>0 / 3</t>
-  </si>
-  <si>
-    <t>65535 / 1</t>
-  </si>
-  <si>
-    <t>65535 / 2</t>
-  </si>
-  <si>
-    <t>65535 / 3</t>
   </si>
 </sst>
 </file>
@@ -613,7 +595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -738,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K8" sqref="K8:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -870,7 +852,7 @@
         <v>12</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>19</v>
@@ -885,7 +867,7 @@
         <v>12</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -902,7 +884,7 @@
         <v>12</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>13</v>
@@ -917,7 +899,7 @@
         <v>12</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -934,7 +916,7 @@
         <v>12</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>20</v>
@@ -949,7 +931,7 @@
         <v>12</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -968,7 +950,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="K8" sqref="K8:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updated TC203 test sheet
</commit_message>
<xml_diff>
--- a/Test Data/TC_203_Verify_If_An_EXI800_Is_Deleted_All_The_IS_Devices_Connected_To_EXI800_Will_Be_Deleted.xlsx
+++ b/Test Data/TC_203_Verify_If_An_EXI800_Is_Deleted_All_The_IS_Devices_Connected_To_EXI800_Will_Be_Deleted.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E029D2-8139-42FB-B33E-20B820D3CD74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" activeTab="1"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Add EXI Devices" sheetId="6" r:id="rId1"/>
@@ -21,18 +22,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="41">
   <si>
     <t>Color Codes</t>
   </si>
@@ -152,12 +147,15 @@
   </si>
   <si>
     <t>VerifyConnectedISDevicesOnEXI</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> To verify connected IS devices on EXI800</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -591,7 +589,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -716,11 +714,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -750,7 +748,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>0</v>
@@ -945,7 +943,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1169,5 +1167,6 @@
     <mergeCell ref="G6:K6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>